<commit_message>
update where files are in code
</commit_message>
<xml_diff>
--- a/outlet-rivers/where_files_are_in_code.xlsx
+++ b/outlet-rivers/where_files_are_in_code.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11015"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/evandethier/satellite-ssc/outlet-rivers/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bowdoin-my.sharepoint.com/personal/e_dethier_bowdoin_edu/Documents/research/satellite-ssc/outlet-rivers/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E150ECA1-D696-BA40-B275-698A9CC50AEE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="19" documentId="13_ncr:1_{E150ECA1-D696-BA40-B275-698A9CC50AEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{14996780-E1A0-9844-A7EC-D09B735ECCBE}"/>
   <bookViews>
-    <workbookView xWindow="1740" yWindow="500" windowWidth="22400" windowHeight="16940" xr2:uid="{AD24723A-B3D3-7C4E-9B77-EFF315FE4D09}"/>
+    <workbookView xWindow="1720" yWindow="500" windowWidth="22400" windowHeight="16940" xr2:uid="{AD24723A-B3D3-7C4E-9B77-EFF315FE4D09}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="73">
   <si>
     <t>File</t>
   </si>
@@ -232,13 +232,25 @@
   </si>
   <si>
     <t>**bolded if not created as part of the code</t>
+  </si>
+  <si>
+    <t>site_band_scaling_all.rds</t>
+  </si>
+  <si>
+    <t>SSC_cluster_function.rds</t>
+  </si>
+  <si>
+    <t>cluster_centers.rds</t>
+  </si>
+  <si>
+    <t>nearby_stns_final.csv</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -618,13 +630,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C9750E3-85A1-E546-A95C-93B691AFEEEA}">
-  <dimension ref="A1:M54"/>
+  <dimension ref="A1:M58"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="65" workbookViewId="0">
-      <selection activeCell="B46" sqref="B46"/>
+      <selection activeCell="A51" activeCellId="6" sqref="A2:A5 A11:A13 A17:A23 A32:A33 A46 A48 A51:A54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="68" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.83203125" style="2" bestFit="1" customWidth="1"/>
@@ -635,7 +647,7 @@
     <col min="14" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="1" customFormat="1" ht="17" thickBot="1">
+    <row r="1" spans="1:13" s="1" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -676,8 +688,8 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:13">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -687,166 +699,157 @@
         <v>64</v>
       </c>
     </row>
-    <row r="3" spans="1:13">
-      <c r="A3" s="2" t="s">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13">
-      <c r="A4" s="2" t="s">
+      <c r="D6" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="K4" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13">
-      <c r="A5" s="2" t="s">
+      <c r="D7" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="K5" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13">
-      <c r="A6" s="2" t="s">
+      <c r="D8" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13">
-      <c r="A7" s="2" t="s">
+      <c r="D9" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D7" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="K7" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13">
-      <c r="A8" s="3" t="s">
+      <c r="D10" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K10" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A11" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B11" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="E8" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13">
-      <c r="A9" s="3" t="s">
+      <c r="E11" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A12" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B12" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="E9" s="3" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13">
-      <c r="A10" s="3" t="s">
+      <c r="E12" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A13" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B13" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="E10" s="3" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13">
-      <c r="A11" s="2" t="s">
+      <c r="E13" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="E11" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13">
-      <c r="A12" s="2" t="s">
+      <c r="E14" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="E12" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13">
-      <c r="A13" s="2" t="s">
+      <c r="E15" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A16" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="E13" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13">
-      <c r="A14" s="3" t="s">
+      <c r="E16" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A17" s="3" t="s">
         <v>26</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="F14" s="3" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13">
-      <c r="A15" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="F15" s="3" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13">
-      <c r="A16" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="F16" s="3" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13">
-      <c r="A17" s="3" t="s">
-        <v>29</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>67</v>
@@ -855,9 +858,9 @@
         <v>64</v>
       </c>
     </row>
-    <row r="18" spans="1:13">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>67</v>
@@ -866,9 +869,9 @@
         <v>64</v>
       </c>
     </row>
-    <row r="19" spans="1:13">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>67</v>
@@ -877,375 +880,419 @@
         <v>64</v>
       </c>
     </row>
-    <row r="20" spans="1:13">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A21" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A22" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A23" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="B23" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="F20" s="3" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13">
-      <c r="A21" s="2" t="s">
+      <c r="F23" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A24" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="F21" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13">
-      <c r="A22" s="2" t="s">
+      <c r="F24" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A25" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="F22" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13">
-      <c r="A23" s="2" t="s">
+      <c r="F25" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A26" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A27" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="F23" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G23" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13">
-      <c r="A24" s="2" t="s">
+      <c r="F27" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A28" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="F24" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G24" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13">
-      <c r="A25" s="2" t="s">
+      <c r="F28" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A29" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="G25" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H25" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="K25" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13">
-      <c r="A26" s="2" t="s">
+      <c r="G29" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H29" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="K29" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A30" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="G26" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H26" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="K26" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13">
-      <c r="A27" s="2" t="s">
+      <c r="G30" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H30" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="K30" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A31" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="G27" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="M27" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13">
-      <c r="A28" s="3" t="s">
+      <c r="G31" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="M31" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A32" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="B28" s="2" t="s">
+      <c r="B32" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="I28" s="3" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13">
-      <c r="A29" s="3" t="s">
+      <c r="I32" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A33" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="B29" s="2" t="s">
+      <c r="B33" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="I29" s="3" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="30" spans="1:13">
-      <c r="A30" s="2" t="s">
+      <c r="I33" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A34" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="H30" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="I30" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="K30" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="31" spans="1:13">
-      <c r="A31" s="2" t="s">
+      <c r="H34" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I34" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="K34" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A35" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="H31" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="I31" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="K31" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="L31" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="32" spans="1:13">
-      <c r="A32" s="2" t="s">
+      <c r="H35" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I35" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="K35" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="L35" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A36" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="H32" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="I32" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="K32" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="L32" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="33" spans="1:13">
-      <c r="A33" s="2" t="s">
+      <c r="H36" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I36" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="K36" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="L36" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A37" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="H33" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="K33" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="34" spans="1:13">
-      <c r="A34" s="2" t="s">
+      <c r="H37" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K37" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A38" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="H34" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="K34" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="M34" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="35" spans="1:13">
-      <c r="A35" s="2" t="s">
+      <c r="H38" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K38" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="M38" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A39" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="H35" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="K35" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="36" spans="1:13">
-      <c r="A36" s="2" t="s">
+      <c r="H39" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K39" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A40" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="H36" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="K36" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="37" spans="1:13">
-      <c r="A37" s="2" t="s">
+      <c r="H40" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K40" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A41" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="H37" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="K37" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="38" spans="1:13">
-      <c r="A38" s="2" t="s">
+      <c r="H41" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K41" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A42" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="H38" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="K38" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="39" spans="1:13">
-      <c r="A39" s="2" t="s">
+      <c r="H42" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K42" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A43" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="H39" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="K39" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="40" spans="1:13">
-      <c r="A40" s="2" t="s">
+      <c r="H43" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K43" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A44" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="H40" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="K40" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="41" spans="1:13">
-      <c r="A41" s="2" t="s">
+      <c r="H44" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K44" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A45" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="I41" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="K41" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="42" spans="1:13">
-      <c r="A42" s="3" t="s">
+      <c r="I45" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K45" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A46" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="B42" s="2" t="s">
+      <c r="B46" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="J42" s="3" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="43" spans="1:13">
-      <c r="A43" s="2" t="s">
+      <c r="J46" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A47" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="J43" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="K43" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="44" spans="1:13">
-      <c r="A44" s="3" t="s">
+      <c r="J47" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K47" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A48" s="3" t="s">
         <v>56</v>
-      </c>
-      <c r="B44" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="K44" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="L44" s="3" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="45" spans="1:13">
-      <c r="A45" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="K45" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="46" spans="1:13">
-      <c r="A46" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="K46" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="47" spans="1:13">
-      <c r="A47" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="B47" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="M47" s="3" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="48" spans="1:13">
-      <c r="A48" s="3" t="s">
-        <v>60</v>
       </c>
       <c r="B48" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="M48" s="3" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="49" spans="1:13">
-      <c r="A49" s="3" t="s">
+      <c r="K48" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="L48" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A49" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="K49" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A50" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="K50" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A51" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="M51" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A52" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="M52" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A53" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="B49" s="2" t="s">
+      <c r="B53" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="M49" s="3" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="50" spans="1:13">
-      <c r="A50" s="3" t="s">
+      <c r="M53" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A54" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="B50" s="2" t="s">
+      <c r="B54" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="M50" s="3" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="51" spans="1:13">
-      <c r="A51" s="2" t="s">
+      <c r="M54" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A55" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="M51" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="54" spans="1:13">
-      <c r="A54" s="4" t="s">
+      <c r="M55" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A58" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="B54" s="3"/>
+      <c r="B58" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>